<commit_message>
commit for fixing comments and register
</commit_message>
<xml_diff>
--- a/app/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/app/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>GitHub (up to 100)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>GithHub Profile Link</t>
@@ -263,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -293,6 +290,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -580,7 +580,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +603,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>10</v>
@@ -612,485 +612,483 @@
         <v>8</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
+      <c r="B3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
+        <v>13</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+        <v>15</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+        <v>12</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="15">
+        <v>5.5</v>
+      </c>
       <c r="D8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="6">
-        <v>5.5</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="15">
+        <v>34</v>
+      </c>
       <c r="D9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="6">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B10" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>12</v>
+      <c r="C11" s="5">
+        <v>5</v>
       </c>
       <c r="D11" s="5">
         <v>10</v>
       </c>
-      <c r="E11" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="5">
+        <v>30</v>
+      </c>
       <c r="D12" s="5">
         <v>30</v>
       </c>
-      <c r="E12" s="5">
-        <v>15</v>
-      </c>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5">
+        <v>5</v>
+      </c>
       <c r="D13" s="5">
         <v>5</v>
       </c>
-      <c r="E13" s="5">
-        <v>5</v>
-      </c>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="C14" s="5">
+        <v>10</v>
+      </c>
       <c r="D14" s="5">
         <v>10</v>
       </c>
-      <c r="E14" s="5">
-        <v>10</v>
-      </c>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="5">
+        <v>5</v>
+      </c>
       <c r="D15" s="5">
         <v>5</v>
       </c>
-      <c r="E15" s="5">
-        <v>5</v>
-      </c>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B16" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="C16" s="5">
+        <v>10</v>
+      </c>
       <c r="D16" s="5">
         <v>10</v>
       </c>
-      <c r="E16" s="5">
-        <v>10</v>
-      </c>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B17" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="C17" s="5">
+        <v>3</v>
+      </c>
       <c r="D17" s="5">
         <v>3</v>
       </c>
-      <c r="E17" s="5">
-        <v>3</v>
-      </c>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B18" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="C18" s="5">
+        <v>7</v>
+      </c>
       <c r="D18" s="5">
         <v>7</v>
       </c>
-      <c r="E18" s="5">
-        <v>7</v>
-      </c>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="C19" s="5">
+        <v>10</v>
+      </c>
       <c r="D19" s="5">
         <v>10</v>
       </c>
-      <c r="E19" s="5">
-        <v>10</v>
-      </c>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="C20" s="5">
+        <v>5</v>
+      </c>
       <c r="D20" s="5">
         <v>5</v>
       </c>
-      <c r="E20" s="5">
-        <v>5</v>
-      </c>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B21" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="C21" s="5">
+        <v>10</v>
+      </c>
       <c r="D21" s="5">
         <v>10</v>
       </c>
-      <c r="E21" s="5">
-        <v>10</v>
-      </c>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="5">
+        <v>10</v>
+      </c>
+      <c r="D22" s="5">
+        <v>10</v>
+      </c>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5">
-        <v>10</v>
-      </c>
-      <c r="E22" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B23" s="13" t="s">
+      <c r="C23" s="5">
+        <v>5</v>
+      </c>
+      <c r="D23" s="5">
+        <v>5</v>
+      </c>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5">
-        <v>5</v>
-      </c>
-      <c r="E23" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B24" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="5">
+        <v>3</v>
+      </c>
       <c r="D24" s="5">
         <v>5</v>
       </c>
-      <c r="E24" s="5">
-        <v>3</v>
-      </c>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="C25" s="5">
+        <v>10</v>
+      </c>
       <c r="D25" s="5">
         <v>10</v>
       </c>
-      <c r="E25" s="5">
-        <v>10</v>
-      </c>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="C26" s="5">
+        <v>10</v>
+      </c>
       <c r="D26" s="5">
         <v>10</v>
       </c>
-      <c r="E26" s="5">
-        <v>10</v>
-      </c>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C27" s="5">
+        <v>10</v>
+      </c>
       <c r="D27" s="5">
         <v>10</v>
       </c>
-      <c r="E27" s="5">
-        <v>10</v>
-      </c>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="C28" s="5">
+        <v>5</v>
+      </c>
       <c r="D28" s="5">
         <v>5</v>
       </c>
-      <c r="E28" s="5">
-        <v>10</v>
-      </c>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="C29" s="5">
+        <v>5</v>
+      </c>
       <c r="D29" s="5">
         <v>5</v>
       </c>
-      <c r="E29" s="5">
-        <v>10</v>
-      </c>
+      <c r="E29" s="5"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="5">
+        <v>10</v>
+      </c>
       <c r="D30" s="5">
         <v>10</v>
       </c>
-      <c r="E30" s="5">
-        <v>10</v>
-      </c>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="C31" s="5">
+        <v>5</v>
+      </c>
       <c r="D31" s="5">
         <v>5</v>
       </c>
-      <c r="E31" s="5">
-        <v>5</v>
-      </c>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="5">
+        <v>5</v>
+      </c>
       <c r="D32" s="5">
         <v>5</v>
       </c>
-      <c r="E32" s="5">
-        <v>5</v>
-      </c>
+      <c r="E32" s="5"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C33" s="5">
+        <v>5</v>
+      </c>
       <c r="D33" s="5">
         <v>5</v>
       </c>
-      <c r="E33" s="5">
-        <v>5</v>
-      </c>
+      <c r="E33" s="5"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C34" s="5">
+        <v>10</v>
+      </c>
       <c r="D34" s="5">
         <v>10</v>
       </c>
-      <c r="E34" s="5">
-        <v>10</v>
-      </c>
+      <c r="E34" s="5"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="C35" s="7">
+        <v>10</v>
+      </c>
       <c r="D35" s="7">
         <v>10</v>
       </c>
-      <c r="E35" s="7">
-        <v>10</v>
-      </c>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="C36" s="7">
+        <v>5</v>
+      </c>
       <c r="D36" s="7">
         <v>5</v>
       </c>
-      <c r="E36" s="7">
-        <v>5</v>
-      </c>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="7"/>
+        <v>29</v>
+      </c>
+      <c r="C37" s="7">
+        <v>10</v>
+      </c>
       <c r="D37" s="7">
         <v>10</v>
       </c>
-      <c r="E37" s="7">
-        <v>10</v>
-      </c>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="C38" s="7">
+        <v>5</v>
+      </c>
       <c r="D38" s="7">
         <v>5</v>
       </c>
-      <c r="E38" s="7">
-        <v>5</v>
-      </c>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="C39" s="7">
+        <v>5</v>
+      </c>
       <c r="D39" s="7">
         <v>5</v>
       </c>
-      <c r="E39" s="7">
-        <v>5</v>
-      </c>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="C40" s="7">
+        <v>5</v>
+      </c>
       <c r="D40" s="7">
         <v>5</v>
       </c>
-      <c r="E40" s="7">
-        <v>5</v>
-      </c>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="7"/>
+        <v>35</v>
+      </c>
+      <c r="C41" s="7">
+        <v>20</v>
+      </c>
       <c r="D41" s="7">
         <v>20</v>
       </c>
-      <c r="E41" s="7">
-        <v>20</v>
-      </c>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C42" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="C42" s="7">
+        <v>10</v>
+      </c>
       <c r="D42" s="7">
         <v>10</v>
       </c>
-      <c r="E42" s="7">
-        <v>10</v>
-      </c>
+      <c r="E42" s="7"/>
     </row>
     <row r="43" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="11">
-        <f>SUM(C6:C42)</f>
-        <v>0</v>
+        <f>SUM(C11:C42)</f>
+        <v>263</v>
       </c>
       <c r="D43" s="11">
         <v>370</v>
       </c>
       <c r="E43" s="1">
         <f>SUM(E11:E42)</f>
-        <v>258</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>